<commit_message>
Balance en Excel con estilos finalizado, falta agrupación
</commit_message>
<xml_diff>
--- a/config/styles.xlsx
+++ b/config/styles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Programación\projects\marx\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C87226-5117-456C-9EC9-8A6E9AA7A043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F19F25-6A33-46D7-A933-5207DC3815B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11604" yWindow="0" windowWidth="11436" windowHeight="12360" xr2:uid="{4EBCED79-6864-4C88-B2AE-8BB2D8767100}"/>
+    <workbookView xWindow="1035" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{4EBCED79-6864-4C88-B2AE-8BB2D8767100}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>h1</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>example</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -78,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +138,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +209,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -232,11 +275,8 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="44" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -265,6 +305,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,18 +655,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92C94EA-E24F-4BE8-942E-3EC8CAC0FF64}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -631,95 +686,123 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="18">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="17">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="12">
-        <v>1000</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="20">
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="19">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1000</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="22">
+      <c r="B6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="21">
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="16">
-        <v>1000</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="24">
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="23">
         <v>1000</v>
       </c>
     </row>

</xml_diff>